<commit_message>
Updated Neural Network based results
Updated Neural Network based results and added the scriptNeuralNet.py
for neural network based experiments.
</commit_message>
<xml_diff>
--- a/Results/Weizmann/Results.xlsx
+++ b/Results/Weizmann/Results.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="24270" windowHeight="12435"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="24270" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SVM" sheetId="1" r:id="rId1"/>
+    <sheet name="NeuralNet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="24">
   <si>
     <t>3D OS DES</t>
   </si>
@@ -75,6 +76,27 @@
   </si>
   <si>
     <t>SVM (-t 0 -b 1) - Linear Kernel</t>
+  </si>
+  <si>
+    <t>Algorithms</t>
+  </si>
+  <si>
+    <t># of hidden Layer = 1</t>
+  </si>
+  <si>
+    <t># of hidden Layer = 2</t>
+  </si>
+  <si>
+    <t># of hidden Layer = 3</t>
+  </si>
+  <si>
+    <t># of hidden Layer = 4</t>
+  </si>
+  <si>
+    <t># of hidden Layer = 5</t>
+  </si>
+  <si>
+    <t># of Hidden Neurons = Vocabulay Size</t>
   </si>
 </sst>
 </file>
@@ -578,11 +600,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U8" sqref="U8"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4074,4 +4096,1503 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AS24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="Q19" sqref="Q19:R19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="45" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:45" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="T1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AC1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AL1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+    </row>
+    <row r="2" spans="1:45" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>250</v>
+      </c>
+      <c r="E3">
+        <v>500</v>
+      </c>
+      <c r="F3">
+        <v>750</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="H3">
+        <v>1250</v>
+      </c>
+      <c r="I3">
+        <v>1500</v>
+      </c>
+      <c r="K3">
+        <v>50</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+      <c r="M3">
+        <v>250</v>
+      </c>
+      <c r="N3">
+        <v>500</v>
+      </c>
+      <c r="O3">
+        <v>750</v>
+      </c>
+      <c r="P3">
+        <v>1000</v>
+      </c>
+      <c r="Q3">
+        <v>1250</v>
+      </c>
+      <c r="R3">
+        <v>1500</v>
+      </c>
+      <c r="T3">
+        <v>50</v>
+      </c>
+      <c r="U3">
+        <v>100</v>
+      </c>
+      <c r="V3">
+        <v>250</v>
+      </c>
+      <c r="W3">
+        <v>500</v>
+      </c>
+      <c r="X3">
+        <v>750</v>
+      </c>
+      <c r="Y3">
+        <v>1000</v>
+      </c>
+      <c r="Z3">
+        <v>1250</v>
+      </c>
+      <c r="AA3">
+        <v>1500</v>
+      </c>
+      <c r="AC3">
+        <v>50</v>
+      </c>
+      <c r="AD3">
+        <v>100</v>
+      </c>
+      <c r="AE3">
+        <v>250</v>
+      </c>
+      <c r="AF3">
+        <v>500</v>
+      </c>
+      <c r="AG3">
+        <v>750</v>
+      </c>
+      <c r="AH3">
+        <v>1000</v>
+      </c>
+      <c r="AI3">
+        <v>1250</v>
+      </c>
+      <c r="AJ3">
+        <v>1500</v>
+      </c>
+      <c r="AL3">
+        <v>50</v>
+      </c>
+      <c r="AM3">
+        <v>100</v>
+      </c>
+      <c r="AN3">
+        <v>250</v>
+      </c>
+      <c r="AO3">
+        <v>500</v>
+      </c>
+      <c r="AP3">
+        <v>750</v>
+      </c>
+      <c r="AQ3">
+        <v>1000</v>
+      </c>
+      <c r="AR3">
+        <v>1250</v>
+      </c>
+      <c r="AS3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>79</v>
+      </c>
+      <c r="C4">
+        <v>88</v>
+      </c>
+      <c r="D4">
+        <v>95</v>
+      </c>
+      <c r="E4">
+        <v>92</v>
+      </c>
+      <c r="F4">
+        <v>93</v>
+      </c>
+      <c r="G4">
+        <v>91</v>
+      </c>
+      <c r="H4">
+        <v>92</v>
+      </c>
+      <c r="I4">
+        <v>91</v>
+      </c>
+      <c r="K4">
+        <v>85.999999639999999</v>
+      </c>
+      <c r="L4">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="M4">
+        <v>95</v>
+      </c>
+      <c r="N4">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="O4">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="P4">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="Q4">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="R4">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="T4">
+        <v>82.000000479999997</v>
+      </c>
+      <c r="U4">
+        <v>89.999999399999993</v>
+      </c>
+      <c r="V4">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="W4">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="X4">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="Y4">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="Z4">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="AA4">
+        <v>10.00000015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>83.000000119999996</v>
+      </c>
+      <c r="C5">
+        <v>92.999999520000003</v>
+      </c>
+      <c r="D5">
+        <v>91.999999880000004</v>
+      </c>
+      <c r="E5">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="F5">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="G5">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="H5">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="I5">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="K5">
+        <v>84.999999399999993</v>
+      </c>
+      <c r="L5">
+        <v>88.999999310000007</v>
+      </c>
+      <c r="M5">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="N5">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="O5">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="P5">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="Q5">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="R5">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="T5">
+        <v>82.999999299999999</v>
+      </c>
+      <c r="U5">
+        <v>86.999999279999997</v>
+      </c>
+      <c r="V5">
+        <v>90.999999340000002</v>
+      </c>
+      <c r="W5">
+        <v>95</v>
+      </c>
+      <c r="X5">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="Y5">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="Z5">
+        <v>95</v>
+      </c>
+      <c r="AA5">
+        <v>10.00000015</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>79.999999849999995</v>
+      </c>
+      <c r="C6">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="D6">
+        <v>95</v>
+      </c>
+      <c r="E6">
+        <v>91.000000009999994</v>
+      </c>
+      <c r="F6">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="G6">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="H6">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="I6">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="K6">
+        <v>78.000000270000001</v>
+      </c>
+      <c r="L6">
+        <v>89.999999399999993</v>
+      </c>
+      <c r="M6">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="N6">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="O6">
+        <v>95</v>
+      </c>
+      <c r="P6">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="Q6">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="R6">
+        <v>89.999999779999996</v>
+      </c>
+      <c r="T6">
+        <v>81.999999880000004</v>
+      </c>
+      <c r="U6">
+        <v>90.000000150000005</v>
+      </c>
+      <c r="V6">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="W6">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="X6">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="Y6">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="Z6">
+        <v>10.00000015</v>
+      </c>
+      <c r="AA6">
+        <v>10.00000015</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>82.999999819999999</v>
+      </c>
+      <c r="C7">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="D7">
+        <v>93.999999759999994</v>
+      </c>
+      <c r="E7">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="F7">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="G7">
+        <v>90.999999639999999</v>
+      </c>
+      <c r="H7">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="I7">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="K7">
+        <v>77.999999669999994</v>
+      </c>
+      <c r="L7">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="M7">
+        <v>90.999999340000002</v>
+      </c>
+      <c r="N7">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="O7">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="P7">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="Q7">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="R7">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="T7">
+        <v>86.999999880000004</v>
+      </c>
+      <c r="U7">
+        <v>89.999999110000005</v>
+      </c>
+      <c r="V7">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="W7">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="X7">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="Y7">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="Z7">
+        <v>91.000000009999994</v>
+      </c>
+      <c r="AA7">
+        <v>94.000000060000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>78.000000420000006</v>
+      </c>
+      <c r="C9">
+        <v>85.000000600000007</v>
+      </c>
+      <c r="D9">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="E9">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="F9">
+        <v>85.99999785</v>
+      </c>
+      <c r="G9">
+        <v>93.999999759999994</v>
+      </c>
+      <c r="H9">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="I9">
+        <v>70.000000749999998</v>
+      </c>
+      <c r="K9">
+        <v>82.000000479999997</v>
+      </c>
+      <c r="L9">
+        <v>88.000000119999996</v>
+      </c>
+      <c r="M9">
+        <v>93.999999759999994</v>
+      </c>
+      <c r="N9">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="O9">
+        <v>93.999999759999994</v>
+      </c>
+      <c r="P9">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="Q9">
+        <v>90.999999340000002</v>
+      </c>
+      <c r="R9">
+        <v>91.999999579999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>76.000000240000006</v>
+      </c>
+      <c r="C10">
+        <v>87.999999520000003</v>
+      </c>
+      <c r="D10">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="E10">
+        <v>93.999999759999994</v>
+      </c>
+      <c r="F10">
+        <v>95</v>
+      </c>
+      <c r="G10">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="H10">
+        <v>91.999999880000004</v>
+      </c>
+      <c r="I10">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="K10">
+        <v>78.999999759999994</v>
+      </c>
+      <c r="L10">
+        <v>90.999999340000002</v>
+      </c>
+      <c r="M10">
+        <v>96.000000240000006</v>
+      </c>
+      <c r="N10">
+        <v>96.000000240000006</v>
+      </c>
+      <c r="O10">
+        <v>92.999999520000003</v>
+      </c>
+      <c r="P10">
+        <v>93.999999759999994</v>
+      </c>
+      <c r="Q10">
+        <v>91.999999880000004</v>
+      </c>
+      <c r="R10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>76.999999579999994</v>
+      </c>
+      <c r="C11">
+        <v>88.999999540000005</v>
+      </c>
+      <c r="D11">
+        <v>95</v>
+      </c>
+      <c r="E11">
+        <v>95</v>
+      </c>
+      <c r="F11">
+        <v>95</v>
+      </c>
+      <c r="G11">
+        <v>95</v>
+      </c>
+      <c r="H11">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="I11">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="K11">
+        <v>80.000000150000005</v>
+      </c>
+      <c r="L11">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="M11">
+        <v>95</v>
+      </c>
+      <c r="N11">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="O11">
+        <v>95</v>
+      </c>
+      <c r="P11">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="Q11">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="R11">
+        <v>94.000000060000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>80</v>
+      </c>
+      <c r="C12">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="E12">
+        <v>95</v>
+      </c>
+      <c r="F12">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="G12">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="H12">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="I12">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="K12">
+        <v>78.000000119999996</v>
+      </c>
+      <c r="L12">
+        <v>95.999999639999999</v>
+      </c>
+      <c r="M12">
+        <v>96.000000240000006</v>
+      </c>
+      <c r="N12">
+        <v>95</v>
+      </c>
+      <c r="O12">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="P12">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="Q12">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="R12">
+        <v>94.000000060000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2"/>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <v>250</v>
+      </c>
+      <c r="E15">
+        <v>500</v>
+      </c>
+      <c r="F15">
+        <v>750</v>
+      </c>
+      <c r="G15">
+        <v>1000</v>
+      </c>
+      <c r="H15">
+        <v>1250</v>
+      </c>
+      <c r="I15">
+        <v>1500</v>
+      </c>
+      <c r="K15">
+        <v>50</v>
+      </c>
+      <c r="L15">
+        <v>100</v>
+      </c>
+      <c r="M15">
+        <v>250</v>
+      </c>
+      <c r="N15">
+        <v>500</v>
+      </c>
+      <c r="O15">
+        <v>750</v>
+      </c>
+      <c r="P15">
+        <v>1000</v>
+      </c>
+      <c r="Q15">
+        <v>1250</v>
+      </c>
+      <c r="R15">
+        <v>1500</v>
+      </c>
+      <c r="T15">
+        <v>50</v>
+      </c>
+      <c r="U15">
+        <v>100</v>
+      </c>
+      <c r="V15">
+        <v>250</v>
+      </c>
+      <c r="W15">
+        <v>500</v>
+      </c>
+      <c r="X15">
+        <v>750</v>
+      </c>
+      <c r="Y15">
+        <v>1000</v>
+      </c>
+      <c r="Z15">
+        <v>1250</v>
+      </c>
+      <c r="AA15">
+        <v>1500</v>
+      </c>
+      <c r="AC15">
+        <v>50</v>
+      </c>
+      <c r="AD15">
+        <v>100</v>
+      </c>
+      <c r="AE15">
+        <v>250</v>
+      </c>
+      <c r="AF15">
+        <v>500</v>
+      </c>
+      <c r="AG15">
+        <v>750</v>
+      </c>
+      <c r="AH15">
+        <v>1000</v>
+      </c>
+      <c r="AI15">
+        <v>1250</v>
+      </c>
+      <c r="AJ15">
+        <v>1500</v>
+      </c>
+      <c r="AL15">
+        <v>50</v>
+      </c>
+      <c r="AM15">
+        <v>100</v>
+      </c>
+      <c r="AN15">
+        <v>250</v>
+      </c>
+      <c r="AO15">
+        <v>500</v>
+      </c>
+      <c r="AP15">
+        <v>750</v>
+      </c>
+      <c r="AQ15">
+        <v>1000</v>
+      </c>
+      <c r="AR15">
+        <v>1250</v>
+      </c>
+      <c r="AS15">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>78.999999759999994</v>
+      </c>
+      <c r="C16">
+        <v>82.999999669999994</v>
+      </c>
+      <c r="D16">
+        <v>88.999999310000007</v>
+      </c>
+      <c r="E16">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="F16">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="G16">
+        <v>95</v>
+      </c>
+      <c r="H16">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="I16">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="K16">
+        <v>85.999999639999999</v>
+      </c>
+      <c r="L16">
+        <v>89.999999700000004</v>
+      </c>
+      <c r="M16">
+        <v>91.999999880000004</v>
+      </c>
+      <c r="N16">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="O16">
+        <v>91.999999880000004</v>
+      </c>
+      <c r="P16">
+        <v>89.999999779999996</v>
+      </c>
+      <c r="Q16">
+        <v>91.999999880000004</v>
+      </c>
+      <c r="R16">
+        <v>92.000000029999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>83.000000119999996</v>
+      </c>
+      <c r="C17">
+        <v>83.99999991</v>
+      </c>
+      <c r="D17">
+        <v>87.999999900000006</v>
+      </c>
+      <c r="E17">
+        <v>96.000000240000006</v>
+      </c>
+      <c r="F17">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="G17">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="H17">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="I17">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="K17">
+        <v>84.999999399999993</v>
+      </c>
+      <c r="L17">
+        <v>86.999999579999994</v>
+      </c>
+      <c r="M17">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="N17">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="O17">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="P17">
+        <v>89.999999779999996</v>
+      </c>
+      <c r="Q17">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="R17">
+        <v>93.000000119999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>79.999999849999995</v>
+      </c>
+      <c r="C18">
+        <v>83.999999169999995</v>
+      </c>
+      <c r="D18">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="E18">
+        <v>90.999999939999995</v>
+      </c>
+      <c r="F18">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="G18">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="H18">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="I18">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="K18">
+        <v>78.000000270000001</v>
+      </c>
+      <c r="L18">
+        <v>85.999999790000004</v>
+      </c>
+      <c r="M18">
+        <v>88.99999991</v>
+      </c>
+      <c r="N18">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="O18">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="P18">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="Q18">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="R18">
+        <v>92.000000029999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>82.999999819999999</v>
+      </c>
+      <c r="C19">
+        <v>88.999999459999998</v>
+      </c>
+      <c r="D19">
+        <v>85</v>
+      </c>
+      <c r="E19">
+        <v>91.999999880000004</v>
+      </c>
+      <c r="F19">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="G19">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="H19">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="I19">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="K19">
+        <v>77.999999669999994</v>
+      </c>
+      <c r="L19">
+        <v>84.999999700000004</v>
+      </c>
+      <c r="M19">
+        <v>87.999999900000006</v>
+      </c>
+      <c r="N19">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="O19">
+        <v>95</v>
+      </c>
+      <c r="P19">
+        <v>91.000000009999994</v>
+      </c>
+      <c r="Q19">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="R19">
+        <v>91.000000009999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>78.000000420000006</v>
+      </c>
+      <c r="C21">
+        <v>76.999999880000004</v>
+      </c>
+      <c r="D21">
+        <v>86.999999880000004</v>
+      </c>
+      <c r="E21">
+        <v>90.999999639999999</v>
+      </c>
+      <c r="F21">
+        <v>94.000000060000005</v>
+      </c>
+      <c r="G21">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="H21">
+        <v>91.999999880000004</v>
+      </c>
+      <c r="I21">
+        <v>89.999999500000001</v>
+      </c>
+      <c r="K21">
+        <v>82.000000479999997</v>
+      </c>
+      <c r="L21">
+        <v>85.999999939999995</v>
+      </c>
+      <c r="M21">
+        <v>85.999999639999999</v>
+      </c>
+      <c r="N21">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="O21">
+        <v>95</v>
+      </c>
+      <c r="P21">
+        <v>91.999999880000004</v>
+      </c>
+      <c r="Q21">
+        <v>89.999999549999998</v>
+      </c>
+      <c r="R21">
+        <v>89.999999549999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>76.000000240000006</v>
+      </c>
+      <c r="C22">
+        <v>80.999999790000004</v>
+      </c>
+      <c r="D22">
+        <v>85.999999939999995</v>
+      </c>
+      <c r="E22">
+        <v>88.999999759999994</v>
+      </c>
+      <c r="F22">
+        <v>88.999999540000005</v>
+      </c>
+      <c r="G22">
+        <v>91.999999880000004</v>
+      </c>
+      <c r="H22">
+        <v>91.999999880000004</v>
+      </c>
+      <c r="I22">
+        <v>91.999999880000004</v>
+      </c>
+      <c r="K22">
+        <v>78.999999759999994</v>
+      </c>
+      <c r="L22">
+        <v>80</v>
+      </c>
+      <c r="M22">
+        <v>84.999999399999993</v>
+      </c>
+      <c r="N22">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="O22">
+        <v>89.999999549999998</v>
+      </c>
+      <c r="P22">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="Q22">
+        <v>90.000000150000005</v>
+      </c>
+      <c r="R22">
+        <v>90.999999790000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>76.999999579999994</v>
+      </c>
+      <c r="C23">
+        <v>86.999999579999994</v>
+      </c>
+      <c r="D23">
+        <v>88.999999759999994</v>
+      </c>
+      <c r="E23">
+        <v>89.999999549999998</v>
+      </c>
+      <c r="F23">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="G23">
+        <v>95</v>
+      </c>
+      <c r="H23">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="I23">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="K23">
+        <v>80.000000150000005</v>
+      </c>
+      <c r="L23">
+        <v>87.99999923</v>
+      </c>
+      <c r="M23">
+        <v>93.999999759999994</v>
+      </c>
+      <c r="N23">
+        <v>91.999999880000004</v>
+      </c>
+      <c r="O23">
+        <v>91.000000240000006</v>
+      </c>
+      <c r="P23">
+        <v>92.999999819999999</v>
+      </c>
+      <c r="Q23">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="R23">
+        <v>93.000000119999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>80</v>
+      </c>
+      <c r="C24">
+        <v>83.99999991</v>
+      </c>
+      <c r="D24">
+        <v>90.999999790000004</v>
+      </c>
+      <c r="E24">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="F24">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="G24">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="H24">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="I24">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="K24">
+        <v>78.000000119999996</v>
+      </c>
+      <c r="L24">
+        <v>81.999999579999994</v>
+      </c>
+      <c r="M24">
+        <v>93.999999759999994</v>
+      </c>
+      <c r="N24">
+        <v>90.000000150000005</v>
+      </c>
+      <c r="O24">
+        <v>95</v>
+      </c>
+      <c r="P24">
+        <v>92.000000029999995</v>
+      </c>
+      <c r="Q24">
+        <v>93.000000119999996</v>
+      </c>
+      <c r="R24">
+        <v>92.000000029999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B14:AS14"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="K1:R1"/>
+    <mergeCell ref="T1:AA1"/>
+    <mergeCell ref="AC1:AJ1"/>
+    <mergeCell ref="AL1:AS1"/>
+    <mergeCell ref="B2:AS2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="T4:AA7">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:R7">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:I7">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T9:AA12">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9:R12">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:I12">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:I19">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:I24">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16:R19">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21:R24">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>